<commit_message>
initial review of metadata tables
</commit_message>
<xml_diff>
--- a/metadata/datatable-metadata.xlsx
+++ b/metadata/datatable-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Downloads/metadata template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/zoe_kanavas_water_ca_gov/Documents/Documents/Water Data Consortium Projects/urban-water-drought-data/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D68CA221-3B16-704B-A5F0-DE6707F29C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{D68CA221-3B16-704B-A5F0-DE6707F29C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EDB0ABC-0F98-4370-8A31-FA1761C71BC1}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34860" yWindow="1920" windowWidth="21600" windowHeight="11295" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="9" r:id="rId1"/>
@@ -25,6 +25,33 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={1EE72051-DB55-443B-B5F5-4A51F092B3C0}</author>
+    <author>tc={8A5F2499-6670-436D-9764-B03F62F6BD41}</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{1EE72051-DB55-443B-B5F5-4A51F092B3C0}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    How is this different from attribute_name?</t>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="1" shapeId="0" xr:uid="{8A5F2499-6670-436D-9764-B03F62F6BD41}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Should we add more stats to this?</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
@@ -80,7 +107,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -93,6 +120,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -230,10 +263,16 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Kanavas, Zoe@DWR (she/her)" id="{49D44100-77C5-4A4A-967C-8B68B218E648}" userId="S::Zoe.Kanavas@water.ca.gov::a9497dc4-3ae7-4325-9eed-74504f04b3ea" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -271,7 +310,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -377,7 +416,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -519,38 +558,49 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D1" dT="2024-07-31T15:58:28.14" personId="{49D44100-77C5-4A4A-967C-8B68B218E648}" id="{1EE72051-DB55-443B-B5F5-4A51F092B3C0}">
+    <text>How is this different from attribute_name?</text>
+  </threadedComment>
+  <threadedComment ref="L1" dT="2024-07-31T16:01:15.73" personId="{49D44100-77C5-4A4A-967C-8B68B218E648}" id="{8A5F2499-6670-436D-9764-B03F62F6BD41}">
+    <text>Should we add more stats to this?</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMG10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="19.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="19.6640625" style="1"/>
+    <col min="1" max="2" width="19.625" style="1"/>
     <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="5.625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="12.125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="14.125" style="3" customWidth="1"/>
     <col min="10" max="10" width="16" style="5" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" style="3" customWidth="1"/>
-    <col min="12" max="13" width="9.1640625" style="5" customWidth="1"/>
-    <col min="14" max="1021" width="19.6640625" style="1"/>
-    <col min="1022" max="1024" width="8.33203125" customWidth="1"/>
+    <col min="11" max="11" width="17.625" style="3" customWidth="1"/>
+    <col min="12" max="13" width="9.125" style="5" customWidth="1"/>
+    <col min="14" max="1021" width="19.625" style="1"/>
+    <col min="1022" max="1024" width="8.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,13 +641,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J2" s="4"/>
       <c r="K2" s="2"/>
       <c r="L2" s="7"/>
     </row>
-    <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G10" s="6"/>
     </row>
   </sheetData>
@@ -620,6 +670,7 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -631,14 +682,14 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="25.125" style="4" customWidth="1"/>
     <col min="3" max="3" width="14" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -649,7 +700,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
additional comments and file restructuring reflecting the 7/31 A/Z discussion; added the attribute label
</commit_message>
<xml_diff>
--- a/metadata/datatable-metadata.xlsx
+++ b/metadata/datatable-metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/zoe_kanavas_water_ca_gov/Documents/Documents/Water Data Consortium Projects/urban-water-drought-data/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{D68CA221-3B16-704B-A5F0-DE6707F29C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EDB0ABC-0F98-4370-8A31-FA1761C71BC1}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{D68CA221-3B16-704B-A5F0-DE6707F29C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D489E7B5-6F8C-4660-97EF-A773189AAE91}"/>
   <bookViews>
-    <workbookView xWindow="34860" yWindow="1920" windowWidth="21600" windowHeight="11295" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-255" windowWidth="29040" windowHeight="15720" tabRatio="834" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    How is this different from attribute_name?</t>
+    How is this different from attribute_name?
+Reply:
+    Describes the data source (UWMP, eAR, etc.)</t>
       </text>
     </comment>
     <comment ref="L1" authorId="1" shapeId="0" xr:uid="{8A5F2499-6670-436D-9764-B03F62F6BD41}">
@@ -52,8 +54,27 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={B4E18447-CEA8-4A46-BFD5-FE0EB100DE43}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{B4E18447-CEA8-4A46-BFD5-FE0EB100DE43}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is where we would define things like the levels of water shortage (i.e. what does a water shortage level of 1 mean?)
+ideally, this definition would be in either the attribute decription column, the methods document, or the values would be recoded to be more self explanatory</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -101,6 +122,12 @@
   </si>
   <si>
     <t>attribute_name</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>mode</t>
   </si>
 </sst>
 </file>
@@ -569,18 +596,30 @@
   <threadedComment ref="D1" dT="2024-07-31T15:58:28.14" personId="{49D44100-77C5-4A4A-967C-8B68B218E648}" id="{1EE72051-DB55-443B-B5F5-4A51F092B3C0}">
     <text>How is this different from attribute_name?</text>
   </threadedComment>
+  <threadedComment ref="D1" dT="2024-07-31T18:06:51.33" personId="{49D44100-77C5-4A4A-967C-8B68B218E648}" id="{8F1138BF-AE5D-4538-9A0E-2397B8118757}" parentId="{1EE72051-DB55-443B-B5F5-4A51F092B3C0}">
+    <text>Describes the data source (UWMP, eAR, etc.)</text>
+  </threadedComment>
   <threadedComment ref="L1" dT="2024-07-31T16:01:15.73" personId="{49D44100-77C5-4A4A-967C-8B68B218E648}" id="{8A5F2499-6670-436D-9764-B03F62F6BD41}">
     <text>Should we add more stats to this?</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2024-07-31T18:13:48.76" personId="{49D44100-77C5-4A4A-967C-8B68B218E648}" id="{B4E18447-CEA8-4A46-BFD5-FE0EB100DE43}">
+    <text>This is where we would define things like the levels of water shortage (i.e. what does a water shortage level of 1 mean?)
+ideally, this definition would be in either the attribute decription column, the methods document, or the values would be recoded to be more self explanatory</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMG10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -600,7 +639,7 @@
     <col min="1022" max="1024" width="8.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -640,14 +679,20 @@
       <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J2" s="4"/>
       <c r="K2" s="2"/>
       <c r="L2" s="7"/>
     </row>
-    <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G10" s="6"/>
     </row>
   </sheetData>
@@ -675,12 +720,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -704,5 +747,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>